<commit_message>
Added rest of the price classes
</commit_message>
<xml_diff>
--- a/resources/kayttotarkoitus-hinnasto.xlsx
+++ b/resources/kayttotarkoitus-hinnasto.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
   <si>
     <t>A</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>999 muualla luokittelemattomat rakennukset</t>
+  </si>
+  <si>
+    <t>ei tiedossa</t>
   </si>
 </sst>
 </file>
@@ -632,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,6 +1264,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
711 teollisuusvarastot = D
</commit_message>
<xml_diff>
--- a/resources/kayttotarkoitus-hinnasto.xlsx
+++ b/resources/kayttotarkoitus-hinnasto.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\lupapiste\lupapiste\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="19335" windowHeight="21780"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="Link00000023" localSheetId="0">Transaktiomaksut!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -344,6 +349,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -391,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -638,7 +646,7 @@
   <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="B63" sqref="A63:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1157,7 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
käyttötarkoitus hinnaston päivitys 711 -> A, 699 -> D, 613 -> D
</commit_message>
<xml_diff>
--- a/resources/kayttotarkoitus-hinnasto.xlsx
+++ b/resources/kayttotarkoitus-hinnasto.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\lupapiste\lupapiste\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joniha/work/lupapiste/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19335" windowHeight="21780"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19340" windowHeight="21780"/>
   </bookViews>
   <sheets>
     <sheet name="Transaktiomaksut" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,11 @@
   <definedNames>
     <definedName name="Link00000023" localSheetId="0">Transaktiomaksut!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -402,9 +405,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -437,9 +440,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -645,18 +648,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B63" sqref="A63:B63"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -664,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -672,7 +675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -680,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -688,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -696,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -704,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -712,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -720,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -728,7 +731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -736,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -744,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -752,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -760,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -768,7 +771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -776,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -784,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -792,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -800,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -808,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -816,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -824,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -832,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -840,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -848,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -856,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -864,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -872,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -880,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -888,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -896,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -904,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -912,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -920,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -928,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -936,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -944,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -952,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -960,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -968,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -976,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -984,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -992,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -1120,15 +1123,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
@@ -1144,23 +1147,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>75</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>77</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>81</v>
       </c>
@@ -1283,10 +1286,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>